<commit_message>
Change in test data file to cover more scenarios
</commit_message>
<xml_diff>
--- a/cypress/fixtures/Fal1-Files/General declaration FAL 1 - goodData.xlsx
+++ b/cypress/fixtures/Fal1-Files/General declaration FAL 1 - goodData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jayanthi\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Homeoffice\NMSW-Main\nmsw-ui\cypress\fixtures\Fal1-Files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC108842-D133-46EF-B27D-080C465FB529}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE9536D-A990-4D65-86AA-0D4EB3F5A909}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4585,8 +4585,8 @@
   </sheetPr>
   <dimension ref="A1:P26"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A6" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="0" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -4670,7 +4670,7 @@
         <v>8</v>
       </c>
       <c r="D5" s="36">
-        <v>44972</v>
+        <v>45049</v>
       </c>
       <c r="E5" s="3" t="s">
         <v>9</v>
@@ -7085,7 +7085,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69140625" defaultRowHeight="15.5" customHeight="1" x14ac:dyDescent="0.35"/>
@@ -7126,14 +7126,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="18390984-f7d9-4502-80ba-82ec344db5fb">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="629dd2dc-abea-47e8-ba88-82202e3ee8ef" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -7374,21 +7372,20 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="18390984-f7d9-4502-80ba-82ec344db5fb">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="629dd2dc-abea-47e8-ba88-82202e3ee8ef" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C2A0AF4-2234-45DE-BCD6-060ACA865D30}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A5056AD-6F82-4433-81E7-2CF7DDF58706}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="18390984-f7d9-4502-80ba-82ec344db5fb"/>
-    <ds:schemaRef ds:uri="629dd2dc-abea-47e8-ba88-82202e3ee8ef"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -7413,9 +7410,12 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3A5056AD-6F82-4433-81E7-2CF7DDF58706}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5C2A0AF4-2234-45DE-BCD6-060ACA865D30}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="18390984-f7d9-4502-80ba-82ec344db5fb"/>
+    <ds:schemaRef ds:uri="629dd2dc-abea-47e8-ba88-82202e3ee8ef"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>